<commit_message>
Ended script for lab 3
</commit_message>
<xml_diff>
--- a/Lab3_ActiveMWDevices/Amplifier_VNA/OpcionalBarridoPotencia.xlsx
+++ b/Lab3_ActiveMWDevices/Amplifier_VNA/OpcionalBarridoPotencia.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\segar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Documents\UPM\MSTC\LRFM\MATLAB\Lab3_ActiveMWDevices\Amplifier_VNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4953F95D-8640-42A3-B4A9-4ECB414AFBC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E71E46DC-5A11-4336-8148-9AE57459FDEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2976" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{9C03E0C6-02A8-40E8-A318-24E39C8B2B88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C03E0C6-02A8-40E8-A318-24E39C8B2B88}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,18 +37,26 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>VNA</t>
+    <t>P_vna</t>
   </si>
   <si>
-    <t>POWER METER</t>
+    <t>P_measured</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,32 +400,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42570C77-64F8-4436-93F2-756703C4BCB2}">
-  <dimension ref="A3:B32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-23</v>
+      </c>
+      <c r="B2">
+        <v>-24.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-22</v>
+      </c>
+      <c r="B3">
+        <v>-23.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-23</v>
+        <v>-21</v>
       </c>
       <c r="B4">
-        <v>-24.13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-22.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-20</v>
       </c>
@@ -423,219 +449,204 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-22</v>
+        <v>-19</v>
       </c>
       <c r="B6">
-        <v>-23.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-19.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-21</v>
+        <v>-18</v>
       </c>
       <c r="B7">
-        <v>-22.09</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-18.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-19</v>
+        <v>-17</v>
       </c>
       <c r="B8">
-        <v>-19.98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-17.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="B9">
-        <v>-18.93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-16.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>-17</v>
+        <v>-15</v>
       </c>
       <c r="B10">
-        <v>-17.87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-15.8</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>-16</v>
+        <v>-14</v>
       </c>
       <c r="B11">
-        <v>-16.84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-14.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="B12">
-        <v>-15.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-13.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="B13">
-        <v>-14.76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-12.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="B14">
-        <v>-13.74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-11.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>-12</v>
+        <v>-10</v>
       </c>
       <c r="B15">
-        <v>-12.71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-10.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-11</v>
+        <v>-9</v>
       </c>
       <c r="B16">
-        <v>-11.68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-9.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="B17">
-        <v>-10.66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-8.65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="B18">
-        <v>-9.65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-7.64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="B19">
-        <v>-8.65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-6.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="B20">
-        <v>-7.64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-5.68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="B21">
-        <v>-6.65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-4.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="B22">
-        <v>-5.68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-3.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="B23">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-2.76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B24">
-        <v>-3.72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-1.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="B25">
-        <v>-2.76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>-0.91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>-1.85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B27">
-        <v>-0.91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1.0649999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29">
-        <v>1.0649999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>2.08</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>3.05</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>5</v>
-      </c>
-      <c r="B32">
         <v>4.0410000000000004</v>
       </c>
     </row>

</xml_diff>